<commit_message>
Finished making all sections populate into excel worksheet. Still need to add years.txt and cadres.txt features
</commit_message>
<xml_diff>
--- a/Python/Indian Police Data Scraping/IPS Data Format.xlsx
+++ b/Python/Indian Police Data Scraping/IPS Data Format.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17440" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17440"/>
   </bookViews>
   <sheets>
     <sheet name="Education" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="128">
   <si>
     <t>dob</t>
   </si>
@@ -281,12 +281,6 @@
   </si>
   <si>
     <t>State in which university located</t>
-  </si>
-  <si>
-    <t>PB-4</t>
-  </si>
-  <si>
-    <t>HY</t>
   </si>
   <si>
     <t>RR</t>
@@ -808,10 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK15"/>
+  <dimension ref="A1:AG15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:AK1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -823,7 +817,7 @@
     <col min="33" max="33" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>66</v>
       </c>
@@ -837,7 +831,7 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -866,77 +860,8 @@
       <c r="N1" t="s">
         <v>34</v>
       </c>
-      <c r="O1" t="s">
-        <v>60</v>
-      </c>
-      <c r="P1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>2</v>
-      </c>
-      <c r="R1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S1" t="s">
-        <v>13</v>
-      </c>
-      <c r="T1" t="s">
-        <v>12</v>
-      </c>
-      <c r="U1" t="s">
-        <v>11</v>
-      </c>
-      <c r="V1" t="s">
-        <v>10</v>
-      </c>
-      <c r="W1" t="s">
-        <v>9</v>
-      </c>
-      <c r="X1" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -967,38 +892,11 @@
       <c r="J2" t="s">
         <v>76</v>
       </c>
-      <c r="O2" t="s">
-        <v>83</v>
-      </c>
-      <c r="P2" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>32013</v>
-      </c>
-      <c r="R2" t="s">
-        <v>85</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2" t="s">
-        <v>87</v>
-      </c>
-      <c r="U2" t="s">
-        <v>89</v>
-      </c>
-      <c r="V2" t="s">
-        <v>91</v>
-      </c>
-      <c r="W2" s="2">
-        <v>35499</v>
-      </c>
-      <c r="X2" s="2">
-        <v>35504</v>
-      </c>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="Q2" s="1"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -1029,38 +927,11 @@
       <c r="J3" t="s">
         <v>76</v>
       </c>
-      <c r="O3" t="s">
-        <v>83</v>
-      </c>
-      <c r="P3" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>32013</v>
-      </c>
-      <c r="R3" t="s">
-        <v>85</v>
-      </c>
-      <c r="S3">
-        <v>2</v>
-      </c>
-      <c r="T3" t="s">
-        <v>87</v>
-      </c>
-      <c r="U3" t="s">
-        <v>90</v>
-      </c>
-      <c r="V3" t="s">
-        <v>92</v>
-      </c>
-      <c r="W3" s="2">
-        <v>35989</v>
-      </c>
-      <c r="X3" s="2">
-        <v>35993</v>
-      </c>
-    </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="Q3" s="1"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>69</v>
       </c>
@@ -1091,38 +962,11 @@
       <c r="J4" t="s">
         <v>76</v>
       </c>
-      <c r="O4" t="s">
-        <v>83</v>
-      </c>
-      <c r="P4" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>32013</v>
-      </c>
-      <c r="R4" t="s">
-        <v>85</v>
-      </c>
-      <c r="S4">
-        <v>3</v>
-      </c>
-      <c r="T4" t="s">
-        <v>87</v>
-      </c>
-      <c r="U4" t="s">
-        <v>89</v>
-      </c>
-      <c r="V4" t="s">
-        <v>92</v>
-      </c>
-      <c r="W4" s="2">
-        <v>36171</v>
-      </c>
-      <c r="X4" s="2">
-        <v>36176</v>
-      </c>
-    </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="Q4" s="1"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -1153,47 +997,11 @@
       <c r="J5" t="s">
         <v>76</v>
       </c>
-      <c r="O5" t="s">
-        <v>83</v>
-      </c>
-      <c r="P5" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>32013</v>
-      </c>
-      <c r="R5" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y5">
-        <v>1</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>101</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>106</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>115</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>117</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>126</v>
-      </c>
-      <c r="AF5" s="2">
-        <v>40849</v>
-      </c>
-      <c r="AG5" s="2">
-        <v>41364</v>
-      </c>
-    </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="Q5" s="1"/>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="2"/>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>69</v>
       </c>
@@ -1224,47 +1032,11 @@
       <c r="J6" t="s">
         <v>76</v>
       </c>
-      <c r="O6" t="s">
-        <v>83</v>
-      </c>
-      <c r="P6" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>32013</v>
-      </c>
-      <c r="R6" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y6">
-        <v>2</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>102</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>115</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>118</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>126</v>
-      </c>
-      <c r="AF6" s="2">
-        <v>36897</v>
-      </c>
-      <c r="AG6" s="2">
-        <v>40848</v>
-      </c>
-    </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="Q6" s="1"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2"/>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -1295,47 +1067,11 @@
       <c r="J7" t="s">
         <v>76</v>
       </c>
-      <c r="O7" t="s">
-        <v>83</v>
-      </c>
-      <c r="P7" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>32013</v>
-      </c>
-      <c r="R7" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y7">
-        <v>3</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>108</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>116</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>118</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>127</v>
-      </c>
-      <c r="AF7" s="2">
-        <v>36892</v>
-      </c>
-      <c r="AG7" s="2">
-        <v>37626</v>
-      </c>
-    </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="Q7" s="1"/>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="2"/>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>69</v>
       </c>
@@ -1366,47 +1102,11 @@
       <c r="J8" t="s">
         <v>76</v>
       </c>
-      <c r="O8" t="s">
-        <v>83</v>
-      </c>
-      <c r="P8" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>32013</v>
-      </c>
-      <c r="R8" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y8">
-        <v>4</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>109</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>116</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>119</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>127</v>
-      </c>
-      <c r="AF8" s="2">
-        <v>36835</v>
-      </c>
-      <c r="AG8" s="2">
-        <v>36891</v>
-      </c>
-    </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="Q8" s="1"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -1437,47 +1137,11 @@
       <c r="J9" t="s">
         <v>76</v>
       </c>
-      <c r="O9" t="s">
-        <v>83</v>
-      </c>
-      <c r="P9" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>32013</v>
-      </c>
-      <c r="R9" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y9">
-        <v>5</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>110</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>116</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>127</v>
-      </c>
-      <c r="AF9" s="2">
-        <v>36435</v>
-      </c>
-      <c r="AG9" s="2">
-        <v>36835</v>
-      </c>
-    </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="Q9" s="1"/>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="2"/>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -1508,44 +1172,11 @@
       <c r="J10" t="s">
         <v>76</v>
       </c>
-      <c r="O10" t="s">
-        <v>83</v>
-      </c>
-      <c r="P10" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q10" s="1">
-        <v>32013</v>
-      </c>
-      <c r="R10" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y10">
-        <v>6</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>111</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>121</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>126</v>
-      </c>
-      <c r="AF10" s="2">
-        <v>35207</v>
-      </c>
-      <c r="AG10" s="2">
-        <v>36435</v>
-      </c>
-    </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="Q10" s="1"/>
+      <c r="AF10" s="2"/>
+      <c r="AG10" s="2"/>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -1576,47 +1207,11 @@
       <c r="J11" t="s">
         <v>76</v>
       </c>
-      <c r="O11" t="s">
-        <v>83</v>
-      </c>
-      <c r="P11" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q11" s="1">
-        <v>32013</v>
-      </c>
-      <c r="R11" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y11">
-        <v>7</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>112</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>116</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>122</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>127</v>
-      </c>
-      <c r="AF11" s="2">
-        <v>34447</v>
-      </c>
-      <c r="AG11" s="2">
-        <v>35206</v>
-      </c>
-    </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="Q11" s="1"/>
+      <c r="AF11" s="2"/>
+      <c r="AG11" s="2"/>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>69</v>
       </c>
@@ -1647,47 +1242,11 @@
       <c r="J12" t="s">
         <v>76</v>
       </c>
-      <c r="O12" t="s">
-        <v>83</v>
-      </c>
-      <c r="P12" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q12" s="1">
-        <v>32013</v>
-      </c>
-      <c r="R12" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y12">
-        <v>8</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>113</v>
-      </c>
-      <c r="AC12" t="s">
-        <v>116</v>
-      </c>
-      <c r="AD12" t="s">
-        <v>123</v>
-      </c>
-      <c r="AE12" t="s">
-        <v>127</v>
-      </c>
-      <c r="AF12" s="2">
-        <v>33418</v>
-      </c>
-      <c r="AG12" s="2">
-        <v>34447</v>
-      </c>
-    </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="Q12" s="1"/>
+      <c r="AF12" s="2"/>
+      <c r="AG12" s="2"/>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -1718,47 +1277,11 @@
       <c r="J13" t="s">
         <v>76</v>
       </c>
-      <c r="O13" t="s">
-        <v>83</v>
-      </c>
-      <c r="P13" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q13" s="1">
-        <v>32013</v>
-      </c>
-      <c r="R13" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y13">
-        <v>9</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>104</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>114</v>
-      </c>
-      <c r="AC13" t="s">
-        <v>116</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>123</v>
-      </c>
-      <c r="AE13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AF13" s="2">
-        <v>32828</v>
-      </c>
-      <c r="AG13" s="2">
-        <v>33417</v>
-      </c>
-    </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="Q13" s="1"/>
+      <c r="AF13" s="2"/>
+      <c r="AG13" s="2"/>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -1789,41 +1312,11 @@
       <c r="J14" t="s">
         <v>76</v>
       </c>
-      <c r="O14" t="s">
-        <v>83</v>
-      </c>
-      <c r="P14" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q14" s="1">
-        <v>32013</v>
-      </c>
-      <c r="R14" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y14">
-        <v>10</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>105</v>
-      </c>
-      <c r="AD14" t="s">
-        <v>124</v>
-      </c>
-      <c r="AE14" t="s">
-        <v>125</v>
-      </c>
-      <c r="AF14" s="2">
-        <v>32013</v>
-      </c>
-      <c r="AG14" s="2">
-        <v>32827</v>
-      </c>
-    </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="Q14" s="1"/>
+      <c r="AF14" s="2"/>
+      <c r="AG14" s="2"/>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -1854,27 +1347,7 @@
       <c r="J15" t="s">
         <v>76</v>
       </c>
-      <c r="O15" t="s">
-        <v>83</v>
-      </c>
-      <c r="P15" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q15" s="1">
-        <v>32013</v>
-      </c>
-      <c r="R15" t="s">
-        <v>85</v>
-      </c>
-      <c r="AH15">
-        <v>1</v>
-      </c>
-      <c r="AI15" t="s">
-        <v>128</v>
-      </c>
-      <c r="AJ15">
-        <v>2004</v>
-      </c>
+      <c r="Q15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1885,8 +1358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1958,13 +1431,13 @@
         <v>23</v>
       </c>
       <c r="U1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="W1" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
@@ -1981,19 +1454,19 @@
         <v>33040</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F2" s="3">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="J2" s="4">
         <v>35499</v>
@@ -2028,19 +1501,19 @@
         <v>33040</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F3" s="3">
         <v>2</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>92</v>
       </c>
       <c r="J3" s="4">
         <v>35989</v>
@@ -2075,19 +1548,19 @@
         <v>33040</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F4" s="3">
         <v>3</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>89</v>
-      </c>
       <c r="I4" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J4" s="4">
         <v>36171</v>
@@ -2122,7 +1595,7 @@
         <v>33040</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -2134,22 +1607,22 @@
         <v>1</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="P5" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q5" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="Q5" s="3" t="s">
-        <v>117</v>
-      </c>
       <c r="R5" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="S5" s="4">
         <v>40849</v>
@@ -2175,7 +1648,7 @@
         <v>33040</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -2187,22 +1660,22 @@
         <v>2</v>
       </c>
       <c r="M6" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="N6" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="O6" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="S6" s="4">
         <v>36897</v>
@@ -2228,7 +1701,7 @@
         <v>33040</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -2240,22 +1713,22 @@
         <v>3</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="P7" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q7" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="Q7" s="3" t="s">
-        <v>118</v>
-      </c>
       <c r="R7" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="S7" s="4">
         <v>36892</v>
@@ -2281,7 +1754,7 @@
         <v>33040</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -2293,22 +1766,22 @@
         <v>4</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="S8" s="4">
         <v>36835</v>
@@ -2334,7 +1807,7 @@
         <v>33040</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -2346,22 +1819,22 @@
         <v>5</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="S9" s="4">
         <v>36435</v>
@@ -2387,7 +1860,7 @@
         <v>33040</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -2399,20 +1872,20 @@
         <v>6</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P10" s="3"/>
       <c r="Q10" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="S10" s="4">
         <v>35207</v>
@@ -2438,7 +1911,7 @@
         <v>33040</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -2450,22 +1923,22 @@
         <v>7</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="S11" s="4">
         <v>34447</v>
@@ -2491,7 +1964,7 @@
         <v>33040</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -2503,22 +1976,22 @@
         <v>8</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="S12" s="4">
         <v>33418</v>
@@ -2544,7 +2017,7 @@
         <v>33040</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -2556,22 +2029,22 @@
         <v>9</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O13" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="P13" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="P13" s="3" t="s">
-        <v>116</v>
-      </c>
       <c r="Q13" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="S13" s="4">
         <v>32828</v>
@@ -2597,7 +2070,7 @@
         <v>33040</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -2609,18 +2082,18 @@
         <v>10</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="S14" s="4">
         <v>32013</v>
@@ -2646,7 +2119,7 @@
         <v>33040</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -2664,7 +2137,7 @@
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
       <c r="U15" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="V15" s="3">
         <v>2004</v>
@@ -2956,7 +2429,7 @@
         <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C20" t="s">
         <v>57</v>
@@ -2978,7 +2451,7 @@
         <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C22" t="s">
         <v>58</v>
@@ -3140,35 +2613,35 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C37" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B38" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" t="s">
         <v>97</v>
-      </c>
-      <c r="C38" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B39" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C39" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>